<commit_message>
CHANGE Miilon - Add more words from pages 55 and 59.
</commit_message>
<xml_diff>
--- a/MiilonData/EditoB2_unite4_p55.xlsx
+++ b/MiilonData/EditoB2_unite4_p55.xlsx
@@ -9,12 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="COMMENTER UN TABLEAU" sheetId="1" r:id="rId1"/>
     <sheet name="INDIQUER UN NOMBRE" sheetId="2" r:id="rId2"/>
     <sheet name="INDIQUER UNE QUANTITÉ" sheetId="3" r:id="rId3"/>
+    <sheet name="INDIQUER UNE FRACTION" sheetId="4" r:id="rId4"/>
+    <sheet name="INDIQUER UNE MAJORITÉ OU UNE MI" sheetId="5" r:id="rId5"/>
+    <sheet name="POUR MODULER UN CHIFFRE" sheetId="6" r:id="rId6"/>
+    <sheet name="POUR COMPARER" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t>Mot français</t>
   </si>
@@ -119,6 +123,102 @@
   </si>
   <si>
     <t>Jestliže sečteme příjmy z roku 2013 a z roku 2014, dostaneme...</t>
+  </si>
+  <si>
+    <t>e~direkt</t>
+  </si>
+  <si>
+    <t>La part des impôts indirects s'est accrue.</t>
+  </si>
+  <si>
+    <t>Podíl nepřímých daní se zvýšil.</t>
+  </si>
+  <si>
+    <t>Les proportions sont respectivement de 27 % et 16 %.</t>
+  </si>
+  <si>
+    <t>Poměry činí 27 % a 16 %.</t>
+  </si>
+  <si>
+    <t>La moitié / le tiers / le quart / un cinquième des Français prend le train.</t>
+  </si>
+  <si>
+    <t>Polovina / třetina / čtvrtina / pětina Francouzů jezdí vlakem.</t>
+  </si>
+  <si>
+    <t>Les deux tiers / les trois quarts des Franciliens ont une voiture.</t>
+  </si>
+  <si>
+    <t>Dvě třetiny / tři čtvrtiny obyvatel Île-de-France (pařížské oblasti) mají auto.</t>
+  </si>
+  <si>
+    <t>Ces voyages représentent 16 % de l'ensemble.</t>
+  </si>
+  <si>
+    <t>Tyto cesty představují 16 % z celku.</t>
+  </si>
+  <si>
+    <t>Plus d'un tiers des Européens, soit 80 millions...</t>
+  </si>
+  <si>
+    <t>Více než jedna třetina Evropanů, totiž 80 milionů...</t>
+  </si>
+  <si>
+    <t>INDIQUER UNE MAJORITÉ OU UNE MINORITÉ</t>
+  </si>
+  <si>
+    <t>La plupart des citadins prennent les transports en commun.</t>
+  </si>
+  <si>
+    <t>Většina obyvatel měst jezdí hromadnou dopravou.</t>
+  </si>
+  <si>
+    <t>La place de la voiture est majoritaire / prépondérante, celle du vélo minoritaire.</t>
+  </si>
+  <si>
+    <t>Pozice automobilů přestavuje většinu / má převahu, pozice kol je v menšině.</t>
+  </si>
+  <si>
+    <t>environ / approximativement un quart</t>
+  </si>
+  <si>
+    <t>asi / přibližně jedna čtvrtina</t>
+  </si>
+  <si>
+    <t>près de / presque la moitié</t>
+  </si>
+  <si>
+    <t>téměř polovina / necelá polovina</t>
+  </si>
+  <si>
+    <t>Par rapport à 2013, la situation de 2014...</t>
+  </si>
+  <si>
+    <t>Oproti roku 2013 je situace v roce 2014...</t>
+  </si>
+  <si>
+    <t>Ils sont 27 %, contre 13 % en 2012.</t>
+  </si>
+  <si>
+    <t>Je jich 27 % oproti 13 % z roku 2012.</t>
+  </si>
+  <si>
+    <t>L'écart entre le chiffre officiel et le nombre réel est important / considérable.</t>
+  </si>
+  <si>
+    <t>Rozdíl mezi oficiálním číslem a skutečným počtem je významný / značný.</t>
+  </si>
+  <si>
+    <t>La différence est minime / faible / négligeable.</t>
+  </si>
+  <si>
+    <t>Rozdíl je nepatrný / slabý / zanedbatelný.</t>
+  </si>
+  <si>
+    <t>La part du train est deux fois plus importante dans les voyages professionnels.</t>
+  </si>
+  <si>
+    <t>Podíl vlakové dopravy je dvakrát významnější u služebních cest.</t>
   </si>
 </sst>
 </file>
@@ -142,7 +242,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,8 +255,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -179,13 +285,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -468,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -638,7 +754,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,4 +842,323 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="str">
+        <f xml:space="preserve"> "{ ""foreign"": """ &amp; A2 &amp; """, ""grammar"": """ &amp; B2 &amp; """, ""pronunciation"": """ &amp; C2 &amp; """, ""meaning"": """ &amp; D2 &amp; """ },"</f>
+        <v>{ "foreign": "La part des impôts indirects s'est accrue.", "grammar": "", "pronunciation": "e~direkt", "meaning": "Podíl nepřímých daní se zvýšil." },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F7" si="0" xml:space="preserve"> "{ ""foreign"": """ &amp; A3 &amp; """, ""grammar"": """ &amp; B3 &amp; """, ""pronunciation"": """ &amp; C3 &amp; """, ""meaning"": """ &amp; D3 &amp; """ },"</f>
+        <v>{ "foreign": "Les proportions sont respectivement de 27 % et 16 %.", "grammar": "", "pronunciation": "", "meaning": "Poměry činí 27 % a 16 %." },</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "La moitié / le tiers / le quart / un cinquième des Français prend le train.", "grammar": "", "pronunciation": "", "meaning": "Polovina / třetina / čtvrtina / pětina Francouzů jezdí vlakem." },</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "Les deux tiers / les trois quarts des Franciliens ont une voiture.", "grammar": "", "pronunciation": "", "meaning": "Dvě třetiny / tři čtvrtiny obyvatel Île-de-France (pařížské oblasti) mají auto." },</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "Ces voyages représentent 16 % de l'ensemble.", "grammar": "", "pronunciation": "", "meaning": "Tyto cesty představují 16 % z celku." },</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "Plus d'un tiers des Européens, soit 80 millions...", "grammar": "", "pronunciation": "", "meaning": "Více než jedna třetina Evropanů, totiž 80 milionů..." },</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="74.140625" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="str">
+        <f xml:space="preserve"> "{ ""foreign"": """ &amp; A2 &amp; """, ""grammar"": """ &amp; B2 &amp; """, ""pronunciation"": """ &amp; C2 &amp; """, ""meaning"": """ &amp; D2 &amp; """ },"</f>
+        <v>{ "foreign": "La plupart des citadins prennent les transports en commun.", "grammar": "", "pronunciation": "", "meaning": "Většina obyvatel měst jezdí hromadnou dopravou." },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="str">
+        <f xml:space="preserve"> "{ ""foreign"": """ &amp; A3 &amp; """, ""grammar"": """ &amp; B3 &amp; """, ""pronunciation"": """ &amp; C3 &amp; """, ""meaning"": """ &amp; D3 &amp; """ },"</f>
+        <v>{ "foreign": "La place de la voiture est majoritaire / prépondérante, celle du vélo minoritaire.", "grammar": "", "pronunciation": "", "meaning": "Pozice automobilů přestavuje většinu / má převahu, pozice kol je v menšině." },</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="73.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="str">
+        <f xml:space="preserve"> "{ ""foreign"": """ &amp; A2 &amp; """, ""grammar"": """ &amp; B2 &amp; """, ""pronunciation"": """ &amp; C2 &amp; """, ""meaning"": """ &amp; D2 &amp; """ },"</f>
+        <v>{ "foreign": "environ / approximativement un quart", "grammar": "", "pronunciation": "", "meaning": "asi / přibližně jedna čtvrtina" },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="str">
+        <f xml:space="preserve"> "{ ""foreign"": """ &amp; A3 &amp; """, ""grammar"": """ &amp; B3 &amp; """, ""pronunciation"": """ &amp; C3 &amp; """, ""meaning"": """ &amp; D3 &amp; """ },"</f>
+        <v>{ "foreign": "près de / presque la moitié", "grammar": "", "pronunciation": "", "meaning": "téměř polovina / necelá polovina" },</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="72.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="str">
+        <f xml:space="preserve"> "{ ""foreign"": """ &amp; A2 &amp; """, ""grammar"": """ &amp; B2 &amp; """, ""pronunciation"": """ &amp; C2 &amp; """, ""meaning"": """ &amp; D2 &amp; """ },"</f>
+        <v>{ "foreign": "Par rapport à 2013, la situation de 2014...", "grammar": "", "pronunciation": "", "meaning": "Oproti roku 2013 je situace v roce 2014..." },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F6" si="0" xml:space="preserve"> "{ ""foreign"": """ &amp; A3 &amp; """, ""grammar"": """ &amp; B3 &amp; """, ""pronunciation"": """ &amp; C3 &amp; """, ""meaning"": """ &amp; D3 &amp; """ },"</f>
+        <v>{ "foreign": "Ils sont 27 %, contre 13 % en 2012.", "grammar": "", "pronunciation": "", "meaning": "Je jich 27 % oproti 13 % z roku 2012." },</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "L'écart entre le chiffre officiel et le nombre réel est important / considérable.", "grammar": "", "pronunciation": "", "meaning": "Rozdíl mezi oficiálním číslem a skutečným počtem je významný / značný." },</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "La différence est minime / faible / négligeable.", "grammar": "", "pronunciation": "", "meaning": "Rozdíl je nepatrný / slabý / zanedbatelný." },</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "La part du train est deux fois plus importante dans les voyages professionnels.", "grammar": "", "pronunciation": "", "meaning": "Podíl vlakové dopravy je dvakrát významnější u služebních cest." },</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>